<commit_message>
Optimization - version 3
</commit_message>
<xml_diff>
--- a/Data_Mappings.xlsx
+++ b/Data_Mappings.xlsx
@@ -8,12 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Dev\SecantOptimiserAPI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{862EE147-82A1-40A1-BFFF-060FA68A9ACF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{351D4C67-06EE-4D94-8AD3-BD9B0D12DCA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{3FD3BC24-FADA-45C0-AE77-19FD57CC5372}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{3FD3BC24-FADA-45C0-AE77-19FD57CC5372}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Request-CUT" sheetId="1" r:id="rId1"/>
+    <sheet name="Request-Stock" sheetId="3" r:id="rId2"/>
+    <sheet name="Response-Job" sheetId="5" r:id="rId3"/>
+    <sheet name="Response-CUT" sheetId="2" r:id="rId4"/>
+    <sheet name="Response-Stock" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,10 +39,341 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="106">
+  <si>
+    <t>Kinetic</t>
+  </si>
+  <si>
+    <t>Secant</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>quantityRequired</t>
+  </si>
+  <si>
+    <t>Overmake</t>
+  </si>
+  <si>
+    <t>overMake</t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Width</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>item.topLength + item.bottomLength</t>
+  </si>
+  <si>
+    <t>mitreWidth</t>
+  </si>
+  <si>
+    <t>Grain</t>
+  </si>
+  <si>
+    <t>grain</t>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>class</t>
+  </si>
+  <si>
+    <t>Identifier</t>
+  </si>
+  <si>
+    <t>identifier</t>
+  </si>
+  <si>
+    <t>Material</t>
+  </si>
+  <si>
+    <t>material</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>Formation</t>
+  </si>
+  <si>
+    <t>formation</t>
+  </si>
+  <si>
+    <t>Stack Height</t>
+  </si>
+  <si>
+    <t>stackHeight</t>
+  </si>
+  <si>
+    <t>Split</t>
+  </si>
+  <si>
+    <t>split</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>Tie H</t>
+  </si>
+  <si>
+    <t>tie</t>
+  </si>
+  <si>
+    <t>Goods Free</t>
+  </si>
+  <si>
+    <t>quantityFree</t>
+  </si>
+  <si>
+    <t>Orig Demand</t>
+  </si>
+  <si>
+    <t>Orig Overmake</t>
+  </si>
+  <si>
+    <t>Edge</t>
+  </si>
+  <si>
+    <t>edge</t>
+  </si>
+  <si>
+    <t>Segment</t>
+  </si>
+  <si>
+    <t>Batch name</t>
+  </si>
+  <si>
+    <t>batch</t>
+  </si>
+  <si>
+    <t>Batches</t>
+  </si>
+  <si>
+    <t>batchLimit</t>
+  </si>
+  <si>
+    <t>Mitre</t>
+  </si>
+  <si>
+    <t>mitreCut</t>
+  </si>
+  <si>
+    <t>mitreType</t>
+  </si>
+  <si>
+    <t>Top Len</t>
+  </si>
+  <si>
+    <t>topLength</t>
+  </si>
+  <si>
+    <t>Bottom Len</t>
+  </si>
+  <si>
+    <t>bottomLength</t>
+  </si>
+  <si>
+    <t>Rear Ang</t>
+  </si>
+  <si>
+    <t>rearAngle</t>
+  </si>
+  <si>
+    <t>Front Ang</t>
+  </si>
+  <si>
+    <t>frontAngle</t>
+  </si>
+  <si>
+    <t>Mitre Width</t>
+  </si>
+  <si>
+    <t>Face</t>
+  </si>
+  <si>
+    <t>Symmetric</t>
+  </si>
+  <si>
+    <t>symmetrical</t>
+  </si>
+  <si>
+    <t>Turn flag</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Gauge</t>
+  </si>
+  <si>
+    <t>Min coil@gauge</t>
+  </si>
+  <si>
+    <t>Max coil@gauge</t>
+  </si>
+  <si>
+    <t>Min inner@diameter</t>
+  </si>
+  <si>
+    <t>Max inner@diameter</t>
+  </si>
+  <si>
+    <t>Min outer@diameter</t>
+  </si>
+  <si>
+    <t>Max outer@diameter</t>
+  </si>
+  <si>
+    <t>Order@weight</t>
+  </si>
+  <si>
+    <t>Max coil@ weight</t>
+  </si>
+  <si>
+    <t>Min process@length</t>
+  </si>
+  <si>
+    <t>Min process@width</t>
+  </si>
+  <si>
+    <t>Max process@length</t>
+  </si>
+  <si>
+    <t>Max process@width</t>
+  </si>
+  <si>
+    <t>Produced@weight</t>
+  </si>
+  <si>
+    <t>Part code</t>
+  </si>
+  <si>
+    <t>Compound</t>
+  </si>
+  <si>
+    <t>Material A</t>
+  </si>
+  <si>
+    <t>Material B</t>
+  </si>
+  <si>
+    <t>Material C</t>
+  </si>
+  <si>
+    <t>Material D</t>
+  </si>
+  <si>
+    <t>Material E</t>
+  </si>
+  <si>
+    <t>lengthInMm</t>
+  </si>
+  <si>
+    <t>widthInMm</t>
+  </si>
+  <si>
+    <t>quantityAvailable</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>Classes</t>
+  </si>
+  <si>
+    <t>Thickness</t>
+  </si>
+  <si>
+    <t>thickness</t>
+  </si>
+  <si>
+    <t>Batch</t>
+  </si>
+  <si>
+    <t>Opened</t>
+  </si>
+  <si>
+    <t>opened</t>
+  </si>
+  <si>
+    <t>Pattern</t>
+  </si>
+  <si>
+    <t>pattern</t>
+  </si>
+  <si>
+    <t>Allocated</t>
+  </si>
+  <si>
+    <t>Job Allocated</t>
+  </si>
+  <si>
+    <t>jobAllocated</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>weight</t>
+  </si>
+  <si>
+    <t>Cost per kg</t>
+  </si>
+  <si>
+    <t>costPerKg</t>
+  </si>
+  <si>
+    <t>N Length</t>
+  </si>
+  <si>
+    <t>N Width</t>
+  </si>
+  <si>
+    <t>Procurement cost</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -66,8 +401,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -382,6 +718,732 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{841F8C35-4888-4AA0-B096-487EB9A3370E}">
+  <dimension ref="A1:C54"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>52</v>
+      </c>
+      <c r="B28" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>54</v>
+      </c>
+      <c r="B29" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>55</v>
+      </c>
+      <c r="C30" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>56</v>
+      </c>
+      <c r="B31" t="s">
+        <v>57</v>
+      </c>
+      <c r="C31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>58</v>
+      </c>
+      <c r="C32" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>59</v>
+      </c>
+      <c r="C33" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>60</v>
+      </c>
+      <c r="C34" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>61</v>
+      </c>
+      <c r="C35" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>62</v>
+      </c>
+      <c r="C36" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>63</v>
+      </c>
+      <c r="C37" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>64</v>
+      </c>
+      <c r="C38" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>65</v>
+      </c>
+      <c r="C39" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>66</v>
+      </c>
+      <c r="C40" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>67</v>
+      </c>
+      <c r="C41" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>68</v>
+      </c>
+      <c r="C42" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>69</v>
+      </c>
+      <c r="C43" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>70</v>
+      </c>
+      <c r="C44" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>71</v>
+      </c>
+      <c r="C45" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>72</v>
+      </c>
+      <c r="C46" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>73</v>
+      </c>
+      <c r="C47" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>74</v>
+      </c>
+      <c r="C48" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>75</v>
+      </c>
+      <c r="C49" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>76</v>
+      </c>
+      <c r="C50" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>77</v>
+      </c>
+      <c r="C51" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>78</v>
+      </c>
+      <c r="C52" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>79</v>
+      </c>
+      <c r="C53" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>80</v>
+      </c>
+      <c r="C54" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DF8266E-2650-4EAC-A589-5574E2642243}">
+  <dimension ref="A1:C27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G18" sqref="G18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.90625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>89</v>
+      </c>
+      <c r="B10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>90</v>
+      </c>
+      <c r="B11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>92</v>
+      </c>
+      <c r="B12" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>94</v>
+      </c>
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>95</v>
+      </c>
+      <c r="B14" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>97</v>
+      </c>
+      <c r="B15" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>99</v>
+      </c>
+      <c r="B16" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>101</v>
+      </c>
+      <c r="B17" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>103</v>
+      </c>
+      <c r="C18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>104</v>
+      </c>
+      <c r="C19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>105</v>
+      </c>
+      <c r="C21" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>59</v>
+      </c>
+      <c r="C22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>76</v>
+      </c>
+      <c r="C23" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>77</v>
+      </c>
+      <c r="C24" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>78</v>
+      </c>
+      <c r="C25" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>79</v>
+      </c>
+      <c r="C26" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>80</v>
+      </c>
+      <c r="C27" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B667635A-C417-4AEF-A29E-DA4B0652927A}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -390,4 +1452,28 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59CB0500-87B7-48B2-AF17-A996DC2672C7}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0D5FA66-5751-4C57-B561-6D08574737DD}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Logic to build response object - Aug 30
</commit_message>
<xml_diff>
--- a/Data_Mappings.xlsx
+++ b/Data_Mappings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Dev\SecantOptimiserAPI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{351D4C67-06EE-4D94-8AD3-BD9B0D12DCA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E2BE170-4BEF-48D1-A9D3-AC8349C5AF50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{3FD3BC24-FADA-45C0-AE77-19FD57CC5372}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{3FD3BC24-FADA-45C0-AE77-19FD57CC5372}"/>
   </bookViews>
   <sheets>
     <sheet name="Request-CUT" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="105">
   <si>
     <t>Kinetic</t>
   </si>
@@ -70,9 +70,6 @@
   </si>
   <si>
     <t>Comments</t>
-  </si>
-  <si>
-    <t>item.topLength + item.bottomLength</t>
   </si>
   <si>
     <t>mitreWidth</t>
@@ -720,9 +717,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{841F8C35-4888-4AA0-B096-487EB9A3370E}">
   <dimension ref="A1:C54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -764,10 +761,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -775,7 +769,7 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
@@ -783,82 +777,82 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
         <v>12</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
         <v>14</v>
-      </c>
-      <c r="B7" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
         <v>16</v>
-      </c>
-      <c r="B8" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
         <v>18</v>
-      </c>
-      <c r="B9" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
         <v>20</v>
-      </c>
-      <c r="B10" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
         <v>22</v>
-      </c>
-      <c r="B11" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" t="s">
         <v>24</v>
-      </c>
-      <c r="B12" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" t="s">
         <v>26</v>
-      </c>
-      <c r="B13" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" t="s">
         <v>28</v>
-      </c>
-      <c r="B14" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" t="s">
         <v>30</v>
-      </c>
-      <c r="B15" t="s">
-        <v>31</v>
       </c>
       <c r="C15" t="s">
         <v>7</v>
@@ -866,10 +860,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" t="s">
         <v>32</v>
-      </c>
-      <c r="B16" t="s">
-        <v>33</v>
       </c>
       <c r="C16" t="s">
         <v>7</v>
@@ -877,7 +871,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C17" t="s">
         <v>7</v>
@@ -885,7 +879,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C18" t="s">
         <v>7</v>
@@ -893,42 +887,42 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" t="s">
         <v>36</v>
-      </c>
-      <c r="B19" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" t="s">
         <v>39</v>
-      </c>
-      <c r="B21" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" t="s">
         <v>41</v>
-      </c>
-      <c r="B22" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" t="s">
         <v>43</v>
-      </c>
-      <c r="B23" t="s">
-        <v>44</v>
       </c>
       <c r="C23" t="s">
         <v>7</v>
@@ -936,10 +930,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C24" t="s">
         <v>7</v>
@@ -947,47 +941,47 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25" t="s">
         <v>46</v>
-      </c>
-      <c r="B25" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26" t="s">
         <v>48</v>
-      </c>
-      <c r="B26" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" t="s">
         <v>50</v>
-      </c>
-      <c r="B27" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28" t="s">
         <v>52</v>
-      </c>
-      <c r="B28" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B29" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C30" t="s">
         <v>7</v>
@@ -995,10 +989,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
+        <v>55</v>
+      </c>
+      <c r="B31" t="s">
         <v>56</v>
-      </c>
-      <c r="B31" t="s">
-        <v>57</v>
       </c>
       <c r="C31" t="s">
         <v>7</v>
@@ -1006,7 +1000,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C32" t="s">
         <v>7</v>
@@ -1014,7 +1008,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C33" t="s">
         <v>7</v>
@@ -1022,7 +1016,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C34" t="s">
         <v>7</v>
@@ -1030,7 +1024,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C35" t="s">
         <v>7</v>
@@ -1038,7 +1032,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C36" t="s">
         <v>7</v>
@@ -1046,7 +1040,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C37" t="s">
         <v>7</v>
@@ -1054,7 +1048,7 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C38" t="s">
         <v>7</v>
@@ -1062,7 +1056,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C39" t="s">
         <v>7</v>
@@ -1070,7 +1064,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C40" t="s">
         <v>7</v>
@@ -1078,7 +1072,7 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C41" t="s">
         <v>7</v>
@@ -1086,7 +1080,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C42" t="s">
         <v>7</v>
@@ -1094,7 +1088,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C43" t="s">
         <v>7</v>
@@ -1102,7 +1096,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C44" t="s">
         <v>7</v>
@@ -1110,7 +1104,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C45" t="s">
         <v>7</v>
@@ -1118,7 +1112,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C46" t="s">
         <v>7</v>
@@ -1126,7 +1120,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C47" t="s">
         <v>7</v>
@@ -1134,7 +1128,7 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C48" t="s">
         <v>7</v>
@@ -1142,7 +1136,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C49" t="s">
         <v>7</v>
@@ -1150,7 +1144,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C50" t="s">
         <v>7</v>
@@ -1158,7 +1152,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C51" t="s">
         <v>7</v>
@@ -1166,7 +1160,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C52" t="s">
         <v>7</v>
@@ -1174,7 +1168,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C53" t="s">
         <v>7</v>
@@ -1182,7 +1176,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C54" t="s">
         <v>7</v>
@@ -1225,7 +1219,7 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
@@ -1236,7 +1230,7 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
@@ -1247,7 +1241,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
@@ -1255,71 +1249,71 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B5" t="s">
         <v>84</v>
-      </c>
-      <c r="B5" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B7" t="s">
         <v>87</v>
-      </c>
-      <c r="B7" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
         <v>16</v>
-      </c>
-      <c r="B8" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
         <v>20</v>
-      </c>
-      <c r="B9" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
+        <v>89</v>
+      </c>
+      <c r="B11" t="s">
         <v>90</v>
-      </c>
-      <c r="B11" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
+        <v>91</v>
+      </c>
+      <c r="B12" t="s">
         <v>92</v>
-      </c>
-      <c r="B12" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C13" t="s">
         <v>7</v>
@@ -1327,39 +1321,39 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
+        <v>94</v>
+      </c>
+      <c r="B14" t="s">
         <v>95</v>
-      </c>
-      <c r="B14" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
+        <v>96</v>
+      </c>
+      <c r="B15" t="s">
         <v>97</v>
-      </c>
-      <c r="B15" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
+        <v>98</v>
+      </c>
+      <c r="B16" t="s">
         <v>99</v>
-      </c>
-      <c r="B16" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
+        <v>100</v>
+      </c>
+      <c r="B17" t="s">
         <v>101</v>
-      </c>
-      <c r="B17" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C18" t="s">
         <v>7</v>
@@ -1367,7 +1361,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C19" t="s">
         <v>7</v>
@@ -1375,15 +1369,15 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" t="s">
         <v>18</v>
-      </c>
-      <c r="B20" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C21" t="s">
         <v>7</v>
@@ -1391,7 +1385,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C22" t="s">
         <v>7</v>
@@ -1399,7 +1393,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C23" t="s">
         <v>7</v>
@@ -1407,7 +1401,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C24" t="s">
         <v>7</v>
@@ -1415,7 +1409,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C25" t="s">
         <v>7</v>
@@ -1423,7 +1417,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C26" t="s">
         <v>7</v>
@@ -1431,7 +1425,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C27" t="s">
         <v>7</v>
@@ -1446,7 +1440,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B667635A-C417-4AEF-A29E-DA4B0652927A}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>

</xml_diff>